<commit_message>
added path to all accession files, using PATH that will be in the cluster file
</commit_message>
<xml_diff>
--- a/targets.xlsx
+++ b/targets.xlsx
@@ -123,96 +123,6 @@
     <t>Stressor</t>
   </si>
   <si>
-    <t>PRJEB6270</t>
-  </si>
-  <si>
-    <t>PRJNA71219</t>
-  </si>
-  <si>
-    <t>PRJNA146329</t>
-  </si>
-  <si>
-    <t>PRJNA154615</t>
-  </si>
-  <si>
-    <t>PRJNA154617</t>
-  </si>
-  <si>
-    <t>PRJNA178077</t>
-  </si>
-  <si>
-    <t>PRJNA182358</t>
-  </si>
-  <si>
-    <t>PRJNA185434</t>
-  </si>
-  <si>
-    <t>PRJNA194079</t>
-  </si>
-  <si>
-    <t>PRJNA194084</t>
-  </si>
-  <si>
-    <t>PRJNA196535</t>
-  </si>
-  <si>
-    <t>PRJNA216134</t>
-  </si>
-  <si>
-    <t>PRJNA217287</t>
-  </si>
-  <si>
-    <t>PRJNA217698</t>
-  </si>
-  <si>
-    <t>PRJNA232734</t>
-  </si>
-  <si>
-    <t>PRJNA232944</t>
-  </si>
-  <si>
-    <t>PRJNA233418</t>
-  </si>
-  <si>
-    <t>PRJNA233528</t>
-  </si>
-  <si>
-    <t>PRJNA233562</t>
-  </si>
-  <si>
-    <t>PRJNA233581</t>
-  </si>
-  <si>
-    <t>PRJNA243050</t>
-  </si>
-  <si>
-    <t>PRJNA281706</t>
-  </si>
-  <si>
-    <t>PRJNA282703</t>
-  </si>
-  <si>
-    <t>PRJNA290387</t>
-  </si>
-  <si>
-    <t>PRJNA291364</t>
-  </si>
-  <si>
-    <t>PRJNA298285</t>
-  </si>
-  <si>
-    <t>PRJNA301543</t>
-  </si>
-  <si>
-    <t>PRJNA316106</t>
-  </si>
-  <si>
-    <t>PRJNA316154</t>
-  </si>
-  <si>
-    <t>PRJNA353875</t>
-  </si>
-  <si>
     <t>BioProjectID</t>
   </si>
   <si>
@@ -234,9 +144,6 @@
     <t>OsHV-1</t>
   </si>
   <si>
-    <t>AccessionFile</t>
-  </si>
-  <si>
     <t>Dry_exposure</t>
   </si>
   <si>
@@ -267,9 +174,6 @@
     <t>Temp_pH</t>
   </si>
   <si>
-    <t>PRJNA167099</t>
-  </si>
-  <si>
     <t>Salinity</t>
   </si>
   <si>
@@ -283,6 +187,102 @@
   </si>
   <si>
     <t>Changes_env_condition</t>
+  </si>
+  <si>
+    <t>AccessionFilePath</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJEB6270.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA71219.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA146329.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA154615.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA154617.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA178077.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA182358.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA185434.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA194079.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA194084.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA196535.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA216134.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA217287.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA217698.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA232734.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA232944.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA233418.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA233528.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA233562.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA233581.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA243050.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA281706.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA282703.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA290387.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA291364.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA298285.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA301543.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA316106.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA316154.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA353875.txt</t>
+  </si>
+  <si>
+    <t>/home/erinroberts/bio_project_data/PRJNA167099.txt</t>
   </si>
 </sst>
 </file>
@@ -725,21 +725,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>33</v>
@@ -756,13 +756,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>271391</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16">
@@ -770,13 +770,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
         <v>71219</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16">
@@ -784,13 +784,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1">
         <v>146329</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16">
@@ -798,13 +798,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1">
         <v>154615</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16">
@@ -812,13 +812,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1">
         <v>154617</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16">
@@ -826,13 +826,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
         <v>178077</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16">
@@ -840,13 +840,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1">
         <v>182358</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16">
@@ -854,13 +854,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1">
         <v>185434</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16">
@@ -868,13 +868,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1">
         <v>194079</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16">
@@ -882,13 +882,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1">
         <v>194084</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16">
@@ -896,13 +896,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1">
         <v>196535</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16">
@@ -910,13 +910,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1">
         <v>216134</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16">
@@ -924,13 +924,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1">
         <v>217287</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16">
@@ -938,13 +938,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1">
         <v>217698</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16">
@@ -952,13 +952,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1">
         <v>232734</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
@@ -966,13 +966,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1">
         <v>232944</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16">
@@ -980,13 +980,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1">
         <v>233418</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16">
@@ -994,13 +994,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1">
         <v>233528</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
@@ -1008,13 +1008,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1">
         <v>233562</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16">
@@ -1022,13 +1022,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>233581</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
@@ -1036,13 +1036,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1">
         <v>243050</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16">
@@ -1050,13 +1050,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1">
         <v>281706</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16">
@@ -1064,13 +1064,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1">
         <v>282703</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16">
@@ -1078,13 +1078,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C25" s="1">
         <v>290387</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
@@ -1092,13 +1092,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1">
         <v>291364</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
@@ -1106,13 +1106,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1">
         <v>298285</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16">
@@ -1120,13 +1120,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1">
         <v>301543</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16">
@@ -1134,13 +1134,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1">
         <v>316106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
@@ -1148,13 +1148,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1">
         <v>316154</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16">
@@ -1162,13 +1162,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1">
         <v>353875</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16">
@@ -1176,13 +1176,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1">
         <v>167099</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>